<commit_message>
Finished the networking list
</commit_message>
<xml_diff>
--- a/Network Contact List 1.0.xlsx
+++ b/Network Contact List 1.0.xlsx
@@ -8,16 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7848b277b5256a99/Desktop/Files/BYU-I/Professional Readiness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="377" documentId="8_{D356B230-0CB4-4248-BE59-F34F1F665A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4FAB649-AF0B-4F54-899A-ED3684B0A443}"/>
+  <xr:revisionPtr revIDLastSave="594" documentId="8_{D356B230-0CB4-4248-BE59-F34F1F665A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDB455AF-B1D3-4E1E-B9B4-5E6EE83D7FE5}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{AE6EC594-1444-43B3-9AD5-706BE80652EF}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" firstSheet="1" activeTab="2" xr2:uid="{AE6EC594-1444-43B3-9AD5-706BE80652EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Network" sheetId="1" r:id="rId1"/>
-    <sheet name="NetworkRsc" sheetId="2" r:id="rId2"/>
+    <sheet name="Network2" sheetId="3" r:id="rId2"/>
+    <sheet name="Network3" sheetId="4" r:id="rId3"/>
+    <sheet name="NetworkRsc" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Network!$B$7:$R$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Network2!$B$7:$R$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Network3!$B$7:$R$27</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="282">
   <si>
     <t>(111) 111-1111</t>
   </si>
@@ -562,6 +566,330 @@
   </si>
   <si>
     <t>CSE Majors</t>
+  </si>
+  <si>
+    <t>Stephen</t>
+  </si>
+  <si>
+    <t>Nelson</t>
+  </si>
+  <si>
+    <t>Calvin</t>
+  </si>
+  <si>
+    <t>Smoot</t>
+  </si>
+  <si>
+    <t>Katie</t>
+  </si>
+  <si>
+    <t>Born</t>
+  </si>
+  <si>
+    <t>Dustin</t>
+  </si>
+  <si>
+    <t>Hill</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Toolson</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>Merrick</t>
+  </si>
+  <si>
+    <t>McCracken</t>
+  </si>
+  <si>
+    <t>Krainock</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>Sosa</t>
+  </si>
+  <si>
+    <t>Vaughn</t>
+  </si>
+  <si>
+    <t>Hazen</t>
+  </si>
+  <si>
+    <t>Micheal</t>
+  </si>
+  <si>
+    <t>Malin</t>
+  </si>
+  <si>
+    <t>Dionne</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Stoddard</t>
+  </si>
+  <si>
+    <t>Christopher</t>
+  </si>
+  <si>
+    <t>Pitts</t>
+  </si>
+  <si>
+    <t>Kari</t>
+  </si>
+  <si>
+    <t>Peck</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Vargas</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Slater</t>
+  </si>
+  <si>
+    <t>Roger</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Pond</t>
+  </si>
+  <si>
+    <t>Dzado</t>
+  </si>
+  <si>
+    <t>Jon</t>
+  </si>
+  <si>
+    <t>Lenenga</t>
+  </si>
+  <si>
+    <t>Ransom</t>
+  </si>
+  <si>
+    <t>Handshake</t>
+  </si>
+  <si>
+    <t>Josh</t>
+  </si>
+  <si>
+    <t>Thieme</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Gay</t>
+  </si>
+  <si>
+    <t>Longhurst</t>
+  </si>
+  <si>
+    <t>Vinitra</t>
+  </si>
+  <si>
+    <t>Muralikrishnan</t>
+  </si>
+  <si>
+    <t>Kolade</t>
+  </si>
+  <si>
+    <t>Ayeni</t>
+  </si>
+  <si>
+    <t>Kendrick</t>
+  </si>
+  <si>
+    <t>Mitchell</t>
+  </si>
+  <si>
+    <t>Arhan</t>
+  </si>
+  <si>
+    <t>Mulay</t>
+  </si>
+  <si>
+    <t>Haskell</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>Justin</t>
+  </si>
+  <si>
+    <t>Salinas</t>
+  </si>
+  <si>
+    <t>Leandra</t>
+  </si>
+  <si>
+    <t>Hall</t>
+  </si>
+  <si>
+    <t>Cornelius</t>
+  </si>
+  <si>
+    <t>Boateng</t>
+  </si>
+  <si>
+    <t>Jeong</t>
+  </si>
+  <si>
+    <t>Covenant</t>
+  </si>
+  <si>
+    <t>Adenuga</t>
+  </si>
+  <si>
+    <t>Louis</t>
+  </si>
+  <si>
+    <t>Muhammad</t>
+  </si>
+  <si>
+    <t>Akhil</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>Quichocho</t>
+  </si>
+  <si>
+    <t>Harshitha</t>
+  </si>
+  <si>
+    <t>Rabala</t>
+  </si>
+  <si>
+    <t>Franklin</t>
+  </si>
+  <si>
+    <t>Lyu</t>
+  </si>
+  <si>
+    <t>Sarthak</t>
+  </si>
+  <si>
+    <t>Gupta</t>
+  </si>
+  <si>
+    <t>Wyatt</t>
+  </si>
+  <si>
+    <t>Holden</t>
+  </si>
+  <si>
+    <t>Catherine</t>
+  </si>
+  <si>
+    <t>Wong</t>
+  </si>
+  <si>
+    <t>Likhitha</t>
+  </si>
+  <si>
+    <t>Mannam</t>
+  </si>
+  <si>
+    <t>Veronika</t>
+  </si>
+  <si>
+    <t>Kitsul</t>
+  </si>
+  <si>
+    <t>Jewel</t>
+  </si>
+  <si>
+    <t>Merriman</t>
+  </si>
+  <si>
+    <t>Evan</t>
+  </si>
+  <si>
+    <t>Bahta</t>
+  </si>
+  <si>
+    <t>Julius</t>
+  </si>
+  <si>
+    <t>Shipton</t>
+  </si>
+  <si>
+    <t>Jingai</t>
+  </si>
+  <si>
+    <t>Liang</t>
+  </si>
+  <si>
+    <t>Pranjal</t>
+  </si>
+  <si>
+    <t>Chalise</t>
+  </si>
+  <si>
+    <t>Mansi</t>
+  </si>
+  <si>
+    <t>Saini</t>
+  </si>
+  <si>
+    <t>Adnan</t>
+  </si>
+  <si>
+    <t>Aman</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>Salazar</t>
+  </si>
+  <si>
+    <t>Carrilo</t>
+  </si>
+  <si>
+    <t>Victor</t>
+  </si>
+  <si>
+    <t>Murta</t>
+  </si>
+  <si>
+    <t>Thoman</t>
+  </si>
+  <si>
+    <t>Wu</t>
+  </si>
+  <si>
+    <t>Blackburn</t>
+  </si>
+  <si>
+    <t>Michelle</t>
+  </si>
+  <si>
+    <t>Chang</t>
+  </si>
+  <si>
+    <t>Zachary</t>
+  </si>
+  <si>
+    <t>Sickles</t>
   </si>
 </sst>
 </file>
@@ -758,7 +1086,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>324851</xdr:rowOff>
     </xdr:to>
@@ -846,6 +1174,282 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2496</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4745E022-E52A-4E34-A5F4-DCD92C3FDCE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="0"/>
+          <a:ext cx="3641046" cy="886279"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>17273</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>342248</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AEAF53A-0CE0-4B01-820B-318DFD432FDD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect l="87921" r="437"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23766273" y="0"/>
+          <a:ext cx="624077" cy="5665201"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>884704</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4233A9EB-2A48-4B4F-B971-4AE1309F318A}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{D14D6069-F61D-4ABA-9B94-FCE7973493E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect t="258" r="464" b="84840"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19439404" y="0"/>
+          <a:ext cx="4950946" cy="913493"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2496</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68021B73-F7F8-4DA7-855B-3D2F709BECCD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="0"/>
+          <a:ext cx="3641046" cy="886279"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>17273</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>342248</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7045942-08E5-4256-8E1B-4C77B9046775}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect l="87921" r="437"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23766273" y="0"/>
+          <a:ext cx="624077" cy="5684077"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>884704</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D831437A-C475-47C5-91EC-1E9C8B82B534}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{D14D6069-F61D-4ABA-9B94-FCE7973493E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect t="258" r="464" b="84840"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19439404" y="0"/>
+          <a:ext cx="4950946" cy="913493"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -888,6 +1492,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1189,8 +1797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46405462-548E-431E-BCAD-3AA0664E3637}">
   <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView showGridLines="0" topLeftCell="A21" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -2172,7 +2780,7 @@
       <c r="Q32" s="7"/>
       <c r="R32" s="7"/>
     </row>
-    <row r="33" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B33" s="4">
         <v>26</v>
       </c>
@@ -2203,7 +2811,7 @@
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
     </row>
-    <row r="34" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B34" s="10">
         <v>27</v>
       </c>
@@ -2234,7 +2842,7 @@
       <c r="Q34" s="7"/>
       <c r="R34" s="7"/>
     </row>
-    <row r="35" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B35" s="4">
         <v>28</v>
       </c>
@@ -2265,7 +2873,7 @@
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
     </row>
-    <row r="36" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B36" s="10">
         <v>29</v>
       </c>
@@ -2296,7 +2904,7 @@
       <c r="Q36" s="7"/>
       <c r="R36" s="7"/>
     </row>
-    <row r="37" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B37" s="4">
         <v>30</v>
       </c>
@@ -2327,7 +2935,7 @@
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
     </row>
-    <row r="38" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B38" s="10">
         <v>31</v>
       </c>
@@ -2358,7 +2966,7 @@
       <c r="Q38" s="7"/>
       <c r="R38" s="7"/>
     </row>
-    <row r="39" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B39" s="4">
         <v>32</v>
       </c>
@@ -2389,7 +2997,7 @@
       <c r="Q39" s="3"/>
       <c r="R39" s="3"/>
     </row>
-    <row r="40" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:18" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B40" s="10">
         <v>33</v>
       </c>
@@ -2420,7 +3028,7 @@
       <c r="Q40" s="7"/>
       <c r="R40" s="7"/>
     </row>
-    <row r="41" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B41" s="4">
         <v>34</v>
       </c>
@@ -2451,10 +3059,7 @@
       <c r="Q41" s="3"/>
       <c r="R41" s="3"/>
     </row>
-    <row r="42" spans="1:18" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>173</v>
-      </c>
+    <row r="42" spans="2:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B42" s="10">
         <v>35</v>
       </c>
@@ -2485,7 +3090,7 @@
       <c r="Q42" s="7"/>
       <c r="R42" s="7"/>
     </row>
-    <row r="43" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B43" s="4">
         <v>36</v>
       </c>
@@ -2516,7 +3121,7 @@
       <c r="Q43" s="3"/>
       <c r="R43" s="3"/>
     </row>
-    <row r="44" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B44" s="10">
         <v>37</v>
       </c>
@@ -2547,7 +3152,7 @@
       <c r="Q44" s="7"/>
       <c r="R44" s="7"/>
     </row>
-    <row r="45" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B45" s="4">
         <v>38</v>
       </c>
@@ -2578,7 +3183,7 @@
       <c r="Q45" s="3"/>
       <c r="R45" s="3"/>
     </row>
-    <row r="46" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B46" s="10">
         <v>39</v>
       </c>
@@ -2609,7 +3214,7 @@
       <c r="Q46" s="7"/>
       <c r="R46" s="7"/>
     </row>
-    <row r="47" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B47" s="4">
         <v>40</v>
       </c>
@@ -2640,7 +3245,7 @@
       <c r="Q47" s="3"/>
       <c r="R47" s="3"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35"/>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.35"/>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O8:O47" xr:uid="{2495CC4D-B976-4F4D-A284-59481D0245A8}">
@@ -2660,6 +3265,2515 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43DAA688-535E-4071-81F1-A6B8746C72BB}">
+  <dimension ref="A1:S48"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="25.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" customWidth="1"/>
+    <col min="8" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="19.1796875" customWidth="1"/>
+    <col min="11" max="11" width="20.26953125" customWidth="1"/>
+    <col min="12" max="12" width="28.1796875" customWidth="1"/>
+    <col min="13" max="13" width="22.26953125" customWidth="1"/>
+    <col min="14" max="14" width="26.7265625" customWidth="1"/>
+    <col min="15" max="15" width="15.81640625" customWidth="1"/>
+    <col min="16" max="16" width="24.453125" customWidth="1"/>
+    <col min="17" max="17" width="16.7265625" customWidth="1"/>
+    <col min="18" max="18" width="33.1796875" customWidth="1"/>
+    <col min="19" max="19" width="9.1796875" customWidth="1"/>
+    <col min="20" max="16384" width="9.1796875" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B7" s="12"/>
+      <c r="C7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="R7" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" s="10">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="11"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="B9" s="4">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="3"/>
+    </row>
+    <row r="10" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="B10" s="10">
+        <v>3</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="7"/>
+    </row>
+    <row r="11" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="B11" s="4">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="3"/>
+    </row>
+    <row r="12" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="B12" s="10">
+        <v>5</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="7"/>
+    </row>
+    <row r="13" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="B13" s="4">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+    </row>
+    <row r="14" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="B14" s="10">
+        <v>7</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+    </row>
+    <row r="15" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="B15" s="4">
+        <v>8</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+    </row>
+    <row r="16" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="B16" s="10">
+        <v>9</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+    </row>
+    <row r="17" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B17" s="4">
+        <v>10</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+    </row>
+    <row r="18" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B18" s="10">
+        <v>11</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+    </row>
+    <row r="19" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B19" s="4">
+        <v>12</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+    </row>
+    <row r="20" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B20" s="10">
+        <v>13</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+    </row>
+    <row r="21" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B21" s="4">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+    </row>
+    <row r="22" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B22" s="10">
+        <v>15</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+    </row>
+    <row r="23" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B23" s="4">
+        <v>16</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+    </row>
+    <row r="24" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B24" s="10">
+        <v>17</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+    </row>
+    <row r="25" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B25" s="4">
+        <v>18</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+    </row>
+    <row r="26" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B26" s="10">
+        <v>19</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+    </row>
+    <row r="27" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B27" s="4">
+        <v>20</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+    </row>
+    <row r="28" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B28" s="10">
+        <v>21</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+    </row>
+    <row r="29" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B29" s="4">
+        <v>22</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+    </row>
+    <row r="30" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>212</v>
+      </c>
+      <c r="B30" s="10">
+        <v>23</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+    </row>
+    <row r="31" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B31" s="4">
+        <v>24</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+    </row>
+    <row r="32" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B32" s="10">
+        <v>25</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+    </row>
+    <row r="33" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B33" s="4">
+        <v>26</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+    </row>
+    <row r="34" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B34" s="10">
+        <v>27</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+    </row>
+    <row r="35" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B35" s="4">
+        <v>28</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E35" s="5"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+    </row>
+    <row r="36" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B36" s="10">
+        <v>29</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+    </row>
+    <row r="37" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B37" s="4">
+        <v>30</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+    </row>
+    <row r="38" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B38" s="10">
+        <v>31</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+    </row>
+    <row r="39" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B39" s="4">
+        <v>32</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="E39" s="5"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+    </row>
+    <row r="40" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B40" s="10">
+        <v>33</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+    </row>
+    <row r="41" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B41" s="4">
+        <v>34</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+    </row>
+    <row r="42" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B42" s="10">
+        <v>35</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="E42" s="8"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
+    </row>
+    <row r="43" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B43" s="4">
+        <v>36</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+    </row>
+    <row r="44" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B44" s="10">
+        <v>37</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="E44" s="8"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="7"/>
+      <c r="Q44" s="7"/>
+      <c r="R44" s="7"/>
+    </row>
+    <row r="45" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B45" s="4">
+        <v>38</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E45" s="5"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
+    </row>
+    <row r="46" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B46" s="10">
+        <v>39</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E46" s="8"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
+      <c r="P46" s="7"/>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="7"/>
+    </row>
+    <row r="47" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B47" s="4">
+        <v>40</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E47" s="5"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G47" xr:uid="{0A91B027-3642-4236-A69F-2257BC2B9FD6}">
+      <formula1>"Text, Phone, Email, LinkedIn, Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O8:O47" xr:uid="{6E684870-98B3-45A3-8813-F204739D9DFD}">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7D1D808-BF34-49EA-873D-ED6CDCB43B26}">
+  <dimension ref="A1:S48"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="25.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" customWidth="1"/>
+    <col min="8" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="19.1796875" customWidth="1"/>
+    <col min="11" max="11" width="20.26953125" customWidth="1"/>
+    <col min="12" max="12" width="28.1796875" customWidth="1"/>
+    <col min="13" max="13" width="22.26953125" customWidth="1"/>
+    <col min="14" max="14" width="26.7265625" customWidth="1"/>
+    <col min="15" max="15" width="15.81640625" customWidth="1"/>
+    <col min="16" max="16" width="24.453125" customWidth="1"/>
+    <col min="17" max="17" width="16.7265625" customWidth="1"/>
+    <col min="18" max="18" width="33.1796875" customWidth="1"/>
+    <col min="19" max="19" width="9.1796875" customWidth="1"/>
+    <col min="20" max="16384" width="9.1796875" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B7" s="12"/>
+      <c r="C7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="R7" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" s="10">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="11"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="B9" s="4">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="3"/>
+    </row>
+    <row r="10" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="B10" s="10">
+        <v>3</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="7"/>
+    </row>
+    <row r="11" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="B11" s="4">
+        <v>4</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="3"/>
+    </row>
+    <row r="12" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="B12" s="10">
+        <v>5</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="7"/>
+    </row>
+    <row r="13" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="B13" s="4">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+    </row>
+    <row r="14" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="B14" s="10">
+        <v>7</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+    </row>
+    <row r="15" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="B15" s="4">
+        <v>8</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+    </row>
+    <row r="16" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="B16" s="10">
+        <v>9</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+    </row>
+    <row r="17" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B17" s="4">
+        <v>10</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+    </row>
+    <row r="18" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B18" s="10">
+        <v>11</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+    </row>
+    <row r="19" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B19" s="4">
+        <v>12</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+    </row>
+    <row r="20" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B20" s="10">
+        <v>13</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+    </row>
+    <row r="21" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B21" s="4">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+    </row>
+    <row r="22" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B22" s="10">
+        <v>15</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+    </row>
+    <row r="23" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B23" s="4">
+        <v>16</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+    </row>
+    <row r="24" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B24" s="10">
+        <v>17</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+    </row>
+    <row r="25" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B25" s="4">
+        <v>18</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+    </row>
+    <row r="26" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B26" s="10">
+        <v>19</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+    </row>
+    <row r="27" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B27" s="4">
+        <v>20</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B28" s="10">
+        <v>21</v>
+      </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B29" s="4">
+        <v>22</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B30" s="10">
+        <v>23</v>
+      </c>
+      <c r="C30" s="10"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B31" s="4">
+        <v>24</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B32" s="10">
+        <v>25</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B33" s="4">
+        <v>26</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B34" s="10">
+        <v>27</v>
+      </c>
+      <c r="C34" s="10"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B35" s="4">
+        <v>28</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B36" s="10">
+        <v>29</v>
+      </c>
+      <c r="C36" s="10"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B37" s="4">
+        <v>30</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B38" s="10">
+        <v>31</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B39" s="4">
+        <v>32</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B40" s="10">
+        <v>33</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B41" s="4">
+        <v>34</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B42" s="10">
+        <v>35</v>
+      </c>
+      <c r="C42" s="10"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B43" s="4">
+        <v>36</v>
+      </c>
+      <c r="C43" s="4"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B44" s="10">
+        <v>37</v>
+      </c>
+      <c r="C44" s="10"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="7"/>
+      <c r="Q44" s="7"/>
+      <c r="R44" s="7"/>
+    </row>
+    <row r="45" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B45" s="4">
+        <v>38</v>
+      </c>
+      <c r="C45" s="4"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B46" s="10">
+        <v>39</v>
+      </c>
+      <c r="C46" s="10"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
+      <c r="P46" s="7"/>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="7"/>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B47" s="4">
+        <v>40</v>
+      </c>
+      <c r="C47" s="4"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O8:O47" xr:uid="{78AD841F-9AB3-47D0-B9C1-4B35A4376FC2}">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G47" xr:uid="{0B9408AC-0350-469A-AF19-0530BC5D0C85}">
+      <formula1>"Text, Phone, Email, LinkedIn, Other"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C0783E-3A71-4FF3-A787-B95C11F0C95B}">
   <dimension ref="A6:I47"/>
   <sheetViews>
@@ -3313,15 +6427,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009A5EC2F65AE6FF4B94F15E1B13D0FB05" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="13aecd974c3bcf9bc12be80b390e7c85">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e08e2f41-3afc-453e-8484-386d79963b73" xmlns:ns3="36043927-bade-4f2e-8132-b7708c18b1e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="00cad41df1e9df714f9d65e01f5175b7" ns2:_="" ns3:_="">
     <xsd:import namespace="e08e2f41-3afc-453e-8484-386d79963b73"/>
@@ -3552,15 +6657,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE01AA14-0DE3-410F-BE0F-F027F102B744}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24D57485-21EB-4728-ADFA-15E030417DC5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3577,4 +6683,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE01AA14-0DE3-410F-BE0F-F027F102B744}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>